<commit_message>
update file added portfolioexample.xlsx 2
</commit_message>
<xml_diff>
--- a/portfolioexample.xlsx
+++ b/portfolioexample.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Oracle</t>
-  </si>
-  <si>
-    <t>QNT</t>
   </si>
   <si>
     <t>MATIC</t>
@@ -401,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +459,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -515,18 +512,18 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>1000</v>
@@ -535,20 +532,6 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>